<commit_message>
Adicionando implementação da api
</commit_message>
<xml_diff>
--- a/metrics/cnn/cnn.xlsx
+++ b/metrics/cnn/cnn.xlsx
@@ -8,19 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\Desktop\prova_2_unidade_bigdata\metrics\cnn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7BB2DC2-BEA1-499F-A709-FCE5E4E78897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD5444FF-C0FA-4641-80C2-B705F7609864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="28800" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21510" yWindow="3735" windowWidth="36000" windowHeight="14385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Acurácia</t>
   </si>
@@ -38,6 +49,9 @@
   </si>
   <si>
     <t>Tempo de classificação</t>
+  </si>
+  <si>
+    <t>Scores</t>
   </si>
 </sst>
 </file>
@@ -93,11 +107,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,9 +415,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -411,6 +428,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -434,22 +452,22 @@
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>0.86324074074074075</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>0.86986722768536373</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>0.86324074074074075</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>0.86007507433398267</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <v>229.4622597694397</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="2">
         <v>0.2465473651885986</v>
       </c>
     </row>
@@ -457,22 +475,22 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>0.88611111111111129</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>0.89241034639968575</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>0.88611111111111129</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>0.88727581064894956</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
         <v>230.51743421554559</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="2">
         <v>0.24531114101409909</v>
       </c>
     </row>
@@ -480,22 +498,22 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>0.87759259259259248</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>0.88259612787456754</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>0.87759259259259248</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>0.87708992474722103</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <v>233.56867752075189</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="2">
         <v>0.27404212951660162</v>
       </c>
     </row>
@@ -503,22 +521,22 @@
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>0.88657407407407407</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>0.89311407782529495</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>0.88657407407407407</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>0.88786673599485311</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
         <v>232.11863176822661</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="2">
         <v>0.24921412467956541</v>
       </c>
     </row>
@@ -526,22 +544,22 @@
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>0.88638888888888889</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>0.89288876449879129</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>0.88638888888888889</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <v>0.88760321664113273</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="2">
         <v>234.788045668602</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="2">
         <v>0.2460354566574097</v>
       </c>
     </row>
@@ -549,22 +567,22 @@
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>0.86527777777777781</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>0.8728739682235187</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <v>0.86527777777777781</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <v>0.86234057371048078</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
         <v>242.8172075033188</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="2">
         <v>0.2598031759262085</v>
       </c>
     </row>
@@ -572,22 +590,22 @@
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>0.88898148148148137</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>0.89617899168512571</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <v>0.88898148148148137</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <v>0.89030552597112733</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2">
         <v>230.40004177093499</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="2">
         <v>0.2437452554702759</v>
       </c>
     </row>
@@ -595,22 +613,22 @@
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>0.88888888888888895</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>0.89511246189491389</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <v>0.88888888888888895</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="2">
         <v>0.89015114801042416</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="2">
         <v>244.4362534046173</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="2">
         <v>0.2579468250274658</v>
       </c>
     </row>
@@ -618,22 +636,22 @@
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2">
         <v>0.88796296296296295</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>0.89676686855785737</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>0.88796296296296295</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <v>0.88982040162905474</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="2">
         <v>248.3710705757141</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="2">
         <v>0.28124730587005609</v>
       </c>
     </row>
@@ -641,22 +659,22 @@
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <v>0.87064814814814806</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>0.87755489650875018</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>0.87064814814814806</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <v>0.86949467524555835</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="2">
         <v>238.83238615989691</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="2">
         <v>0.2479229688644409</v>
       </c>
     </row>
@@ -664,22 +682,22 @@
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="2">
         <v>0.8787962962962963</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="2">
         <v>0.88544457375570218</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="2">
         <v>0.8787962962962963</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="2">
         <v>0.87881714902537433</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="2">
         <v>239.55973668098451</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="2">
         <v>0.25828094482421882</v>
       </c>
     </row>
@@ -687,22 +705,22 @@
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="2">
         <v>0.88027777777777771</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="2">
         <v>0.88858143743696361</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="2">
         <v>0.88027777777777771</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="2">
         <v>0.88045637984405845</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="2">
         <v>260.30706920623783</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="2">
         <v>0.27366261482238768</v>
       </c>
     </row>
@@ -710,22 +728,22 @@
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="2">
         <v>0.88824074074074066</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="2">
         <v>0.89488004484627726</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="2">
         <v>0.88824074074074066</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="2">
         <v>0.8897012306130696</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="2">
         <v>257.10275831222532</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="2">
         <v>0.26583690643310548</v>
       </c>
     </row>
@@ -733,22 +751,22 @@
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="2">
         <v>0.88898148148148159</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="2">
         <v>0.89580984413208176</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="2">
         <v>0.88898148148148159</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="2">
         <v>0.89021151171328672</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="2">
         <v>294.86011657714852</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="2">
         <v>0.28819007873535157</v>
       </c>
     </row>
@@ -756,22 +774,22 @@
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="2">
         <v>0.88120370370370371</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="2">
         <v>0.88387347136489003</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="2">
         <v>0.88120370370370371</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="2">
         <v>0.88026803117352426</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="2">
         <v>269.1112855434418</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="2">
         <v>0.29958565235137941</v>
       </c>
     </row>
@@ -779,22 +797,22 @@
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="2">
         <v>0.88509259259259265</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="2">
         <v>0.89400834614861346</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="2">
         <v>0.88509259259259265</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="2">
         <v>0.88689450862608388</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="2">
         <v>255.3243507862091</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="2">
         <v>0.26753950119018549</v>
       </c>
     </row>
@@ -802,22 +820,22 @@
       <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="2">
         <v>0.87342592592592594</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="2">
         <v>0.87654564091000431</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="2">
         <v>0.87342592592592594</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="2">
         <v>0.87184892617397414</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="2">
         <v>265.63092408180239</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="2">
         <v>0.27225306034088143</v>
       </c>
     </row>
@@ -825,22 +843,22 @@
       <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="2">
         <v>0.8778703703703703</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="2">
         <v>0.88323845757821984</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="2">
         <v>0.8778703703703703</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="2">
         <v>0.87813374163515101</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="2">
         <v>256.48704984188078</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="2">
         <v>0.26189637184143072</v>
       </c>
     </row>
@@ -848,22 +866,22 @@
       <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="2">
         <v>0.87305555555555558</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="2">
         <v>0.88110175133237245</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="2">
         <v>0.87305555555555558</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="2">
         <v>0.87200238174373745</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="2">
         <v>259.81123995780939</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="2">
         <v>0.27533130645751952</v>
       </c>
     </row>
@@ -871,22 +889,22 @@
       <c r="A21" s="1">
         <v>19</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="2">
         <v>0.88611111111111107</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="2">
         <v>0.89349370629811597</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="2">
         <v>0.88611111111111107</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="2">
         <v>0.88737150881933857</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="2">
         <v>264.23931124210361</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="2">
         <v>0.27261319160461428</v>
       </c>
     </row>
@@ -894,22 +912,22 @@
       <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="2">
         <v>0.87231481481481477</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="2">
         <v>0.87703868999692303</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="2">
         <v>0.87231481481481477</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="2">
         <v>0.87083730379031576</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="2">
         <v>254.9387110948563</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="2">
         <v>0.29399602413177489</v>
       </c>
     </row>
@@ -917,22 +935,22 @@
       <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="2">
         <v>0.86898148148148147</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="2">
         <v>0.8772723083718903</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="2">
         <v>0.86898148148148147</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="2">
         <v>0.8666186977311876</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="2">
         <v>249.92667930126191</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="2">
         <v>0.25411546230316162</v>
       </c>
     </row>
@@ -940,22 +958,22 @@
       <c r="A24" s="1">
         <v>22</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="2">
         <v>0.89111111111111119</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="2">
         <v>0.89657532912509708</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="2">
         <v>0.89111111111111119</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="2">
         <v>0.89219327708291407</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="2">
         <v>264.31538362503051</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="2">
         <v>0.27114160060882569</v>
       </c>
     </row>
@@ -963,22 +981,22 @@
       <c r="A25" s="1">
         <v>23</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="2">
         <v>0.88796296296296295</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="2">
         <v>0.89409259150044917</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="2">
         <v>0.88796296296296295</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="2">
         <v>0.88916503637745448</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="2">
         <v>261.3012433052063</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="2">
         <v>0.27040674686431893</v>
       </c>
     </row>
@@ -986,22 +1004,22 @@
       <c r="A26" s="1">
         <v>24</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="2">
         <v>0.87555555555555542</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="2">
         <v>0.8816338846526518</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="2">
         <v>0.87555555555555542</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="2">
         <v>0.87528601820743668</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="2">
         <v>258.84759712219238</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="2">
         <v>0.27256648540496831</v>
       </c>
     </row>
@@ -1009,22 +1027,22 @@
       <c r="A27" s="1">
         <v>25</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="2">
         <v>0.88666666666666671</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="2">
         <v>0.89305969625984072</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="2">
         <v>0.88666666666666671</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="2">
         <v>0.88773770798299745</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="2">
         <v>249.42153949737551</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="2">
         <v>0.26058547496795648</v>
       </c>
     </row>
@@ -1032,22 +1050,22 @@
       <c r="A28" s="1">
         <v>26</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="2">
         <v>0.88925925925925919</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="2">
         <v>0.89433554862236964</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="2">
         <v>0.88925925925925919</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="2">
         <v>0.8902973189797716</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="2">
         <v>256.33768191337577</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="2">
         <v>0.29417386054992678</v>
       </c>
     </row>
@@ -1055,22 +1073,22 @@
       <c r="A29" s="1">
         <v>27</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="2">
         <v>0.87027777777777771</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="2">
         <v>0.87595141101825647</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="2">
         <v>0.87027777777777771</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="2">
         <v>0.87009074316637736</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="2">
         <v>264.52164525985722</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="2">
         <v>0.27939372062683099</v>
       </c>
     </row>
@@ -1078,22 +1096,22 @@
       <c r="A30" s="1">
         <v>28</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="2">
         <v>0.8899999999999999</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="2">
         <v>0.89558227622531861</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="2">
         <v>0.8899999999999999</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="2">
         <v>0.89110267572120794</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="2">
         <v>261.48846247196201</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="2">
         <v>0.27377049922943109</v>
       </c>
     </row>
@@ -1101,26 +1119,56 @@
       <c r="A31" s="1">
         <v>29</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="2">
         <v>0.87351851851851836</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="2">
         <v>0.88152243623655691</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="2">
         <v>0.87351851851851836</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="2">
         <v>0.87307931793618221</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="2">
         <v>254.37119958400729</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="2">
         <v>0.26253457069396968</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="2">
+        <f>AVERAGE(B2:B31)</f>
+        <v>0.8806790123456788</v>
+      </c>
+      <c r="C32" s="2">
+        <f>AVERAGE(C2:C31)</f>
+        <v>0.88711350589888183</v>
+      </c>
+      <c r="D32" s="2">
+        <f>AVERAGE(D2:D31)</f>
+        <v>0.8806790123456788</v>
+      </c>
+      <c r="E32" s="2">
+        <f>AVERAGE(E2:E31)</f>
+        <v>0.88080455177587424</v>
+      </c>
+      <c r="F32" s="2">
+        <f>AVERAGE(F2:F31)</f>
+        <v>252.10719979206715</v>
+      </c>
+      <c r="G32" s="2">
+        <f>AVERAGE(G2:G31)</f>
+        <v>0.26732299407323201</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>